<commit_message>
Added outlines and adjusted marker size
</commit_message>
<xml_diff>
--- a/DataRefValue.xlsx
+++ b/DataRefValue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJENNI01\dev\RVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A7F220-ADEC-4D27-B9D2-7F79FB7F155C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8822C2F2-7F6B-48A4-A162-760B773360DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="60" windowWidth="14610" windowHeight="15585" xr2:uid="{F35416F2-6AE6-41D6-8D54-D88B766F1951}"/>
+    <workbookView xWindow="2805" yWindow="3345" windowWidth="14400" windowHeight="11985" xr2:uid="{F35416F2-6AE6-41D6-8D54-D88B766F1951}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="100">
   <si>
     <t>AEGL-1</t>
   </si>
@@ -324,6 +324,18 @@
   </si>
   <si>
     <t>Beige</t>
+  </si>
+  <si>
+    <t>Outline</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Circle-Open</t>
   </si>
 </sst>
 </file>
@@ -526,13 +538,6 @@
     <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{52FD969E-4BC3-473D-A85B-E39CD8EB1077}"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="52"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -761,6 +766,13 @@
       </font>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="52"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -775,24 +787,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E75E4B-5090-4C16-85F8-1BBCFC676D7C}" name="Table1" displayName="Table1" ref="A1:Q61" totalsRowShown="0">
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E75E4B-5090-4C16-85F8-1BBCFC676D7C}" name="Table1" displayName="Table1" ref="A1:R61" totalsRowShown="0">
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{765B223E-3008-4C65-8D7D-45FF98AB70EB}" name="RefValue"/>
-    <tableColumn id="2" xr3:uid="{FF36F16C-63A9-4B0E-B348-50CE6E8F3348}" name="Value1" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{CBBD1EDB-F02C-47C0-B15E-BE36D2FE9648}" name="Duration1" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{3079463E-09D8-4A1C-B1F4-F64E1FD3D336}" name="Value2" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{0BB7A341-10B1-49AF-9A6A-8306A01E5441}" name="Duration2" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{8C60ABEA-0804-4A7D-8B7D-DED7A96073C7}" name="Value3" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{99F76B4C-4F8E-468A-BADA-AB9B5D93F737}" name="Duration3" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{A3885031-02FB-4552-8611-CFC64B5B2633}" name="Value4" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{2BE87C06-EFFC-4951-AD28-A159B0262DF5}" name="Duration4" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{99F37FBF-F17A-4ED8-9A1A-D1018D6C8E88}" name="Value5" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{0F306807-BE7B-4C46-BDE3-B18D6716ADCC}" name="Duration5" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{FE2371C7-8873-42BB-AE5A-CC5250563E6F}" name="Value6" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{16B48072-AFE2-46DF-9B63-EF74C4CF0784}" name="Duration6" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{FF36F16C-63A9-4B0E-B348-50CE6E8F3348}" name="Value1" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CBBD1EDB-F02C-47C0-B15E-BE36D2FE9648}" name="Duration1" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{3079463E-09D8-4A1C-B1F4-F64E1FD3D336}" name="Value2" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{0BB7A341-10B1-49AF-9A6A-8306A01E5441}" name="Duration2" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{8C60ABEA-0804-4A7D-8B7D-DED7A96073C7}" name="Value3" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{99F76B4C-4F8E-468A-BADA-AB9B5D93F737}" name="Duration3" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{A3885031-02FB-4552-8611-CFC64B5B2633}" name="Value4" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{2BE87C06-EFFC-4951-AD28-A159B0262DF5}" name="Duration4" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{99F37FBF-F17A-4ED8-9A1A-D1018D6C8E88}" name="Value5" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{0F306807-BE7B-4C46-BDE3-B18D6716ADCC}" name="Duration5" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{FE2371C7-8873-42BB-AE5A-CC5250563E6F}" name="Value6" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{16B48072-AFE2-46DF-9B63-EF74C4CF0784}" name="Duration6" dataDxfId="0"/>
     <tableColumn id="14" xr3:uid="{4219645A-4D76-4DA2-B85F-72220C65416F}" name="Type"/>
     <tableColumn id="17" xr3:uid="{272B79C2-042E-4C75-A891-D4C436F04E82}" name="Shape"/>
     <tableColumn id="19" xr3:uid="{15F1B65F-F07A-4C27-92CE-F8ADE102388D}" name="MarkColor"/>
+    <tableColumn id="16" xr3:uid="{D2B739B8-699C-42F5-84C4-0913B1A1FDEC}" name="Outline"/>
     <tableColumn id="15" xr3:uid="{F0CD5FB6-E7CE-4F4C-9F21-D9A1E164DCC8}" name="CatColor"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1096,32 +1109,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F21B303-626C-4027-B174-49D25BE7A0DE}">
-  <dimension ref="A1:T61"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J20" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25:O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="14"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="14"/>
-    <col min="5" max="5" width="11.1796875" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="14"/>
-    <col min="7" max="7" width="11.1796875" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="14"/>
-    <col min="9" max="9" width="11.1796875" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="14"/>
-    <col min="11" max="11" width="11.1796875" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="14"/>
-    <col min="13" max="13" width="11.1796875" customWidth="1"/>
-    <col min="14" max="16" width="21.453125" customWidth="1"/>
-    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="14"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="14"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="14"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="14"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="14"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="14"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="17" width="21.42578125" customWidth="1"/>
+    <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>60</v>
       </c>
@@ -1171,10 +1184,13 @@
         <v>86</v>
       </c>
       <c r="Q1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1217,16 +1233,19 @@
         <v>81</v>
       </c>
       <c r="P2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1272,13 +1291,16 @@
         <v>87</v>
       </c>
       <c r="Q3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R3" t="s">
         <v>74</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1321,16 +1343,19 @@
         <v>81</v>
       </c>
       <c r="P4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="Q4" t="s">
+        <v>97</v>
+      </c>
+      <c r="R4" t="s">
         <v>74</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1360,10 +1385,13 @@
         <v>74</v>
       </c>
       <c r="Q5" t="s">
+        <v>97</v>
+      </c>
+      <c r="R5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1393,10 +1421,13 @@
         <v>87</v>
       </c>
       <c r="Q6" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1426,10 +1457,13 @@
         <v>88</v>
       </c>
       <c r="Q7" t="s">
+        <v>97</v>
+      </c>
+      <c r="R7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1455,10 +1489,13 @@
         <v>74</v>
       </c>
       <c r="Q8" t="s">
+        <v>97</v>
+      </c>
+      <c r="R8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1484,10 +1521,13 @@
         <v>87</v>
       </c>
       <c r="Q9" t="s">
+        <v>97</v>
+      </c>
+      <c r="R9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1513,10 +1553,13 @@
         <v>88</v>
       </c>
       <c r="Q10" t="s">
+        <v>97</v>
+      </c>
+      <c r="R10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1542,10 +1585,13 @@
         <v>74</v>
       </c>
       <c r="Q11" t="s">
+        <v>97</v>
+      </c>
+      <c r="R11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1571,10 +1617,13 @@
         <v>75</v>
       </c>
       <c r="Q12" t="s">
+        <v>97</v>
+      </c>
+      <c r="R12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1600,10 +1649,13 @@
         <v>93</v>
       </c>
       <c r="Q13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1633,10 +1685,13 @@
         <v>93</v>
       </c>
       <c r="Q14" t="s">
+        <v>97</v>
+      </c>
+      <c r="R14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1666,10 +1721,13 @@
         <v>75</v>
       </c>
       <c r="Q15" t="s">
+        <v>97</v>
+      </c>
+      <c r="R15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1699,10 +1757,13 @@
         <v>94</v>
       </c>
       <c r="Q16" t="s">
+        <v>97</v>
+      </c>
+      <c r="R16" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1732,10 +1793,13 @@
         <v>74</v>
       </c>
       <c r="Q17" t="s">
+        <v>97</v>
+      </c>
+      <c r="R17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1769,10 +1833,13 @@
         <v>93</v>
       </c>
       <c r="Q18" t="s">
+        <v>97</v>
+      </c>
+      <c r="R18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1806,10 +1873,13 @@
         <v>75</v>
       </c>
       <c r="Q19" t="s">
+        <v>97</v>
+      </c>
+      <c r="R19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1835,10 +1905,13 @@
         <v>95</v>
       </c>
       <c r="Q20" t="s">
+        <v>97</v>
+      </c>
+      <c r="R20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1872,10 +1945,13 @@
         <v>95</v>
       </c>
       <c r="Q21" t="s">
+        <v>97</v>
+      </c>
+      <c r="R21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1901,10 +1977,13 @@
         <v>95</v>
       </c>
       <c r="Q22" t="s">
+        <v>97</v>
+      </c>
+      <c r="R22" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1934,10 +2013,13 @@
         <v>94</v>
       </c>
       <c r="Q23" t="s">
+        <v>97</v>
+      </c>
+      <c r="R23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1969,10 +2051,13 @@
         <v>75</v>
       </c>
       <c r="Q24" t="s">
+        <v>97</v>
+      </c>
+      <c r="R24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1996,16 +2081,19 @@
         <v>78</v>
       </c>
       <c r="O25" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="P25" t="s">
         <v>74</v>
       </c>
       <c r="Q25" t="s">
+        <v>98</v>
+      </c>
+      <c r="R25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2029,16 +2117,19 @@
         <v>78</v>
       </c>
       <c r="O26" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="P26" t="s">
         <v>87</v>
       </c>
       <c r="Q26" t="s">
+        <v>98</v>
+      </c>
+      <c r="R26" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2074,16 +2165,19 @@
         <v>78</v>
       </c>
       <c r="O27" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="P27" t="s">
         <v>88</v>
       </c>
       <c r="Q27" t="s">
+        <v>98</v>
+      </c>
+      <c r="R27" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -2117,10 +2211,13 @@
         <v>91</v>
       </c>
       <c r="Q28" t="s">
+        <v>97</v>
+      </c>
+      <c r="R28" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2150,10 +2247,13 @@
         <v>89</v>
       </c>
       <c r="Q29" t="s">
+        <v>97</v>
+      </c>
+      <c r="R29" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -2203,10 +2303,13 @@
         <v>88</v>
       </c>
       <c r="Q30" t="s">
+        <v>97</v>
+      </c>
+      <c r="R30" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>29</v>
       </c>
@@ -2236,10 +2339,13 @@
         <v>90</v>
       </c>
       <c r="Q31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>30</v>
       </c>
@@ -2269,10 +2375,13 @@
         <v>90</v>
       </c>
       <c r="Q32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -2306,10 +2415,13 @@
         <v>90</v>
       </c>
       <c r="Q33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
@@ -2343,10 +2455,13 @@
         <v>90</v>
       </c>
       <c r="Q34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -2380,10 +2495,13 @@
         <v>76</v>
       </c>
       <c r="Q35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
@@ -2417,10 +2535,13 @@
         <v>76</v>
       </c>
       <c r="Q36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
@@ -2454,10 +2575,13 @@
         <v>90</v>
       </c>
       <c r="Q37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>36</v>
       </c>
@@ -2487,10 +2611,13 @@
         <v>76</v>
       </c>
       <c r="Q38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>37</v>
       </c>
@@ -2520,10 +2647,13 @@
         <v>76</v>
       </c>
       <c r="Q39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
@@ -2558,10 +2688,13 @@
         <v>76</v>
       </c>
       <c r="Q40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>39</v>
       </c>
@@ -2587,10 +2720,13 @@
         <v>92</v>
       </c>
       <c r="Q41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
@@ -2620,10 +2756,13 @@
         <v>92</v>
       </c>
       <c r="Q42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>41</v>
       </c>
@@ -2657,10 +2796,13 @@
         <v>92</v>
       </c>
       <c r="Q43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
@@ -2694,10 +2836,13 @@
         <v>92</v>
       </c>
       <c r="Q44" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>43</v>
       </c>
@@ -2731,10 +2876,13 @@
         <v>92</v>
       </c>
       <c r="Q45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>44</v>
       </c>
@@ -2764,10 +2912,13 @@
         <v>76</v>
       </c>
       <c r="Q46" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>45</v>
       </c>
@@ -2793,10 +2944,13 @@
         <v>76</v>
       </c>
       <c r="Q47" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>46</v>
       </c>
@@ -2826,10 +2980,13 @@
         <v>76</v>
       </c>
       <c r="Q48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>47</v>
       </c>
@@ -2864,10 +3021,13 @@
         <v>76</v>
       </c>
       <c r="Q49" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>48</v>
       </c>
@@ -2893,10 +3053,13 @@
         <v>76</v>
       </c>
       <c r="Q50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>49</v>
       </c>
@@ -2946,10 +3109,13 @@
         <v>76</v>
       </c>
       <c r="Q51" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
@@ -2983,10 +3149,13 @@
         <v>76</v>
       </c>
       <c r="Q52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>51</v>
       </c>
@@ -3036,10 +3205,13 @@
         <v>76</v>
       </c>
       <c r="Q53" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>52</v>
       </c>
@@ -3089,10 +3261,13 @@
         <v>76</v>
       </c>
       <c r="Q54" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>53</v>
       </c>
@@ -3142,10 +3317,13 @@
         <v>76</v>
       </c>
       <c r="Q55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>54</v>
       </c>
@@ -3179,10 +3357,13 @@
         <v>76</v>
       </c>
       <c r="Q56" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -3216,10 +3397,13 @@
         <v>90</v>
       </c>
       <c r="Q57" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="R57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>56</v>
       </c>
@@ -3253,10 +3437,13 @@
         <v>88</v>
       </c>
       <c r="Q58" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>57</v>
       </c>
@@ -3290,10 +3477,13 @@
         <v>87</v>
       </c>
       <c r="Q59" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>58</v>
       </c>
@@ -3328,10 +3518,13 @@
         <v>76</v>
       </c>
       <c r="Q60" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="R60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>59</v>
       </c>
@@ -3366,19 +3559,22 @@
         <v>89</v>
       </c>
       <c r="Q61" t="s">
+        <v>98</v>
+      </c>
+      <c r="R61" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="A57:A61">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N61" xr:uid="{B44BD58F-F7D2-4008-8040-6723F35A00A3}">
-      <formula1>$T$2:$T$4</formula1>
+      <formula1>$U$2:$U$4</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>